<commit_message>
added tests related to customer
</commit_message>
<xml_diff>
--- a/src/data/testData.xlsx
+++ b/src/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Space\workspace\vscode-workspace\protractor-sample\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF15A7B4-5CD6-4C2A-AF28-2ECA6491570E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D705E9-2CAD-45FB-93EA-A1D6C2B26C7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Pound</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Customer added successfully with customer id</t>
+  </si>
+  <si>
+    <t>Account created successfully with account Number</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,16 +130,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -413,22 +442,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +475,11 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -459,8 +493,11 @@
         <v>560094</v>
       </c>
       <c r="E2" s="2"/>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -472,8 +509,11 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -483,6 +523,9 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>